<commit_message>
Uploaded 17-Jan-2019 10:50:25 {/src/main/resources/com/myspace/shipping_quote/Determine Shipping Price Distance Based.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/shipping_quote/Determine Shipping Price Distance Based.xlsx
+++ b/src/main/resources/com/myspace/shipping_quote/Determine Shipping Price Distance Based.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium – Large</t>
   </si>
   <si>
     <t xml:space="preserve">Large</t>
@@ -179,7 +182,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
@@ -300,10 +303,24 @@
         <v>300</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>3000</v>
+        <v>450</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>450</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>